<commit_message>
feat(cronograma): evidências (upload/download/excluir), popup de nova tarefa, dropdown Título/Tarefa com estilização, campo de progresso (%) e suporte de backend ao campo tipo e ao armazenamento de evidências
</commit_message>
<xml_diff>
--- a/front-end/dist/Base de dados.xlsx
+++ b/front-end/dist/Base de dados.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edyne\OneDrive\Desktop\Assets Life\front-end\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507B718-6936-43B8-BD7A-142A2C52885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA78209E-A07D-49C2-BF34-3902F8E618D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{34F9AA7E-928B-44DE-B956-EFFEEB32D3C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34F9AA7E-928B-44DE-B956-EFFEEB32D3C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nº Imobilizado</t>
   </si>
@@ -42,46 +42,49 @@
     <t>Sub Nº</t>
   </si>
   <si>
-    <t>data inicio da depreciação</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Valor Aquisição</t>
-  </si>
-  <si>
-    <t>Depreciação Acum.</t>
-  </si>
-  <si>
-    <t>Valor contábil</t>
-  </si>
-  <si>
     <t>Centro Custos</t>
   </si>
   <si>
     <t>Classe</t>
   </si>
   <si>
-    <t>Conta Contábil</t>
-  </si>
-  <si>
     <t>Desc. Conta Contabil</t>
   </si>
   <si>
-    <t>Vida útil (anos)</t>
-  </si>
-  <si>
-    <t>Vida útil (períodos)</t>
-  </si>
-  <si>
-    <t>Data fim depreciação</t>
-  </si>
-  <si>
     <t>Auxiliar 1</t>
   </si>
   <si>
     <t>Auxiliar 2</t>
+  </si>
+  <si>
+    <t>Desc. Classe</t>
+  </si>
+  <si>
+    <t>Vida Util (anos)</t>
+  </si>
+  <si>
+    <t>Vida Util (períodos)</t>
+  </si>
+  <si>
+    <t>Data Inicio da Depreciacao</t>
+  </si>
+  <si>
+    <t>Descricao</t>
+  </si>
+  <si>
+    <t>Valor Aquisicao</t>
+  </si>
+  <si>
+    <t>Depreciacao Acum.</t>
+  </si>
+  <si>
+    <t>Valor Contabil</t>
+  </si>
+  <si>
+    <t>Conta Contabil</t>
+  </si>
+  <si>
+    <t>Data Fim Depreciacao</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B343FB1-8EBA-49CE-949A-41CF482BCDEC}">
-  <dimension ref="A1:P1"/>
+  <sheetPr codeName="Planilha1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,14 +454,15 @@
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,46 +470,49 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>